<commit_message>
Boost Containers option and clang fixes.
</commit_message>
<xml_diff>
--- a/LRUCacheTestResults.xlsx
+++ b/LRUCacheTestResults.xlsx
@@ -4,17 +4,21 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="9303"/>
   <workbookPr defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="96" yWindow="36" windowWidth="3780" windowHeight="2160" activeTab="1"/>
+    <workbookView xWindow="96" yWindow="36" windowWidth="3780" windowHeight="2160" activeTab="4"/>
   </bookViews>
   <sheets>
     <sheet name="Test Description" sheetId="1" r:id="rId1"/>
     <sheet name="Sequence #1" sheetId="4" r:id="rId2"/>
     <sheet name="Sequence #2" sheetId="2" r:id="rId3"/>
     <sheet name="Sheet1" sheetId="5" r:id="rId4"/>
+    <sheet name="Sequence #1 (2016.12.20)" sheetId="6" r:id="rId5"/>
+    <sheet name="Sequence #2 (2016.12.20)" sheetId="8" r:id="rId6"/>
   </sheets>
   <definedNames>
     <definedName name="_1_x86" localSheetId="1">'Sequence #1'!$A$6:$C$21</definedName>
+    <definedName name="_1_x86" localSheetId="4">'Sequence #1 (2016.12.20)'!$A$7:$C$22</definedName>
     <definedName name="_1_x86" localSheetId="2">'Sequence #2'!$A$6:$C$21</definedName>
+    <definedName name="_1_x86" localSheetId="5">'Sequence #2 (2016.12.20)'!$A$7:$C$22</definedName>
   </definedNames>
   <calcPr calcId="145621"/>
 </workbook>
@@ -40,11 +44,29 @@
       </textFields>
     </textPr>
   </connection>
+  <connection id="3" name="1_x862" type="6" refreshedVersion="4" background="1" saveData="1">
+    <textPr codePage="866" firstRow="2" sourceFile="E:\MyBoostExperiments\LRUCacheTest\1_x86.csv" tab="0" comma="1">
+      <textFields count="3">
+        <textField/>
+        <textField/>
+        <textField/>
+      </textFields>
+    </textPr>
+  </connection>
+  <connection id="4" name="1_x8621" type="6" refreshedVersion="4" background="1" saveData="1">
+    <textPr codePage="866" firstRow="2" sourceFile="E:\MyBoostExperiments\LRUCacheTest\1_x86.csv" tab="0" comma="1">
+      <textFields count="3">
+        <textField/>
+        <textField/>
+        <textField/>
+      </textFields>
+    </textPr>
+  </connection>
 </connections>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="132" uniqueCount="50">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="240" uniqueCount="55">
   <si>
     <t>The LRUCacheTest is a project comparing performance of different implementations of cache with LRU replacement policies</t>
   </si>
@@ -193,7 +215,22 @@
     <t>The second test sequence results summary:</t>
   </si>
   <si>
-    <t>Test Name, Average Running time(ms), Average Absolute Running Time Deviation(ms)</t>
+    <t>Av. Time(ms)</t>
+  </si>
+  <si>
+    <t>Std.Dev.</t>
+  </si>
+  <si>
+    <t>boost::hash</t>
+  </si>
+  <si>
+    <t>boost::hash &amp; boost::containers</t>
+  </si>
+  <si>
+    <t>Test Name, Average Running time(ms), Standard Deviation(ms)</t>
+  </si>
+  <si>
+    <t>The first test sequence results summary:</t>
   </si>
 </sst>
 </file>
@@ -238,7 +275,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="13">
+  <cellXfs count="14">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="left"/>
@@ -264,13 +301,16 @@
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="left" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment horizontal="left"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -292,6 +332,14 @@
 
 <file path=xl/queryTables/queryTable2.xml><?xml version="1.0" encoding="utf-8"?>
 <queryTable xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" name="1_x86" connectionId="2" autoFormatId="16" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="1" applyPatternFormats="1" applyAlignmentFormats="0" applyWidthHeightFormats="0"/>
+</file>
+
+<file path=xl/queryTables/queryTable3.xml><?xml version="1.0" encoding="utf-8"?>
+<queryTable xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" name="1_x86" connectionId="3" autoFormatId="16" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="1" applyPatternFormats="1" applyAlignmentFormats="0" applyWidthHeightFormats="0"/>
+</file>
+
+<file path=xl/queryTables/queryTable4.xml><?xml version="1.0" encoding="utf-8"?>
+<queryTable xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" name="1_x86" connectionId="4" autoFormatId="16" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="1" applyPatternFormats="1" applyAlignmentFormats="0" applyWidthHeightFormats="0"/>
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
@@ -597,34 +645,34 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:11" s="1" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="A1" s="12" t="s">
+      <c r="A1" s="10" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="12"/>
-      <c r="C1" s="12"/>
-      <c r="D1" s="12"/>
-      <c r="E1" s="12"/>
-      <c r="F1" s="12"/>
-      <c r="G1" s="12"/>
-      <c r="H1" s="12"/>
-      <c r="I1" s="12"/>
-      <c r="J1" s="12"/>
-      <c r="K1" s="12"/>
+      <c r="B1" s="10"/>
+      <c r="C1" s="10"/>
+      <c r="D1" s="10"/>
+      <c r="E1" s="10"/>
+      <c r="F1" s="10"/>
+      <c r="G1" s="10"/>
+      <c r="H1" s="10"/>
+      <c r="I1" s="10"/>
+      <c r="J1" s="10"/>
+      <c r="K1" s="10"/>
     </row>
     <row r="2" spans="1:11" ht="73.8" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A2" s="11" t="s">
+      <c r="A2" s="13" t="s">
         <v>46</v>
       </c>
-      <c r="B2" s="11"/>
-      <c r="C2" s="11"/>
-      <c r="D2" s="11"/>
-      <c r="E2" s="11"/>
-      <c r="F2" s="11"/>
-      <c r="G2" s="11"/>
-      <c r="H2" s="11"/>
-      <c r="I2" s="11"/>
-      <c r="J2" s="11"/>
-      <c r="K2" s="11"/>
+      <c r="B2" s="13"/>
+      <c r="C2" s="13"/>
+      <c r="D2" s="13"/>
+      <c r="E2" s="13"/>
+      <c r="F2" s="13"/>
+      <c r="G2" s="13"/>
+      <c r="H2" s="13"/>
+      <c r="I2" s="13"/>
+      <c r="J2" s="13"/>
+      <c r="K2" s="13"/>
     </row>
     <row r="3" spans="1:11" ht="29.4" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A3" s="2"/>
@@ -664,36 +712,36 @@
       <c r="A5" s="5" t="s">
         <v>6</v>
       </c>
-      <c r="B5" s="9" t="s">
+      <c r="B5" s="11" t="s">
         <v>1</v>
       </c>
-      <c r="C5" s="9"/>
-      <c r="D5" s="9" t="s">
+      <c r="C5" s="11"/>
+      <c r="D5" s="11" t="s">
         <v>14</v>
       </c>
-      <c r="E5" s="9"/>
+      <c r="E5" s="11"/>
     </row>
     <row r="6" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A6" s="5" t="s">
         <v>7</v>
       </c>
-      <c r="B6" s="9" t="s">
+      <c r="B6" s="11" t="s">
         <v>2</v>
       </c>
-      <c r="C6" s="9"/>
-      <c r="D6" s="9"/>
-      <c r="E6" s="9"/>
+      <c r="C6" s="11"/>
+      <c r="D6" s="11"/>
+      <c r="E6" s="11"/>
     </row>
     <row r="7" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A7" s="5" t="s">
         <v>3</v>
       </c>
-      <c r="B7" s="9">
+      <c r="B7" s="11">
         <v>16000000</v>
       </c>
-      <c r="C7" s="9"/>
-      <c r="D7" s="9"/>
-      <c r="E7" s="9"/>
+      <c r="C7" s="11"/>
+      <c r="D7" s="11"/>
+      <c r="E7" s="11"/>
     </row>
     <row r="8" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A8" s="5" t="s">
@@ -767,40 +815,40 @@
       <c r="A12" s="5" t="s">
         <v>15</v>
       </c>
-      <c r="B12" s="9">
+      <c r="B12" s="11">
         <v>2048</v>
       </c>
-      <c r="C12" s="9"/>
-      <c r="D12" s="9">
+      <c r="C12" s="11"/>
+      <c r="D12" s="11">
         <v>65536</v>
       </c>
-      <c r="E12" s="9"/>
+      <c r="E12" s="11"/>
     </row>
     <row r="13" spans="1:11" ht="55.2" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A13" s="5" t="s">
         <v>16</v>
       </c>
-      <c r="B13" s="10" t="s">
+      <c r="B13" s="12" t="s">
         <v>17</v>
       </c>
-      <c r="C13" s="10"/>
-      <c r="D13" s="10" t="s">
+      <c r="C13" s="12"/>
+      <c r="D13" s="12" t="s">
         <v>18</v>
       </c>
-      <c r="E13" s="10"/>
+      <c r="E13" s="12"/>
     </row>
   </sheetData>
   <mergeCells count="10">
+    <mergeCell ref="B12:C12"/>
+    <mergeCell ref="D12:E12"/>
+    <mergeCell ref="B13:C13"/>
+    <mergeCell ref="D13:E13"/>
+    <mergeCell ref="A2:K2"/>
     <mergeCell ref="A1:K1"/>
     <mergeCell ref="B5:C5"/>
     <mergeCell ref="D5:E5"/>
     <mergeCell ref="B6:E6"/>
     <mergeCell ref="B7:E7"/>
-    <mergeCell ref="B12:C12"/>
-    <mergeCell ref="D12:E12"/>
-    <mergeCell ref="B13:C13"/>
-    <mergeCell ref="D13:E13"/>
-    <mergeCell ref="A2:K2"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
@@ -811,7 +859,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:O21"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="F21" sqref="F21"/>
     </sheetView>
   </sheetViews>
@@ -828,88 +876,88 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:15" x14ac:dyDescent="0.3">
-      <c r="B1" s="9" t="s">
+      <c r="B1" s="11" t="s">
         <v>44</v>
       </c>
-      <c r="C1" s="9"/>
-      <c r="D1" s="9"/>
-      <c r="E1" s="9"/>
+      <c r="C1" s="11"/>
+      <c r="D1" s="11"/>
+      <c r="E1" s="11"/>
       <c r="F1" s="8"/>
       <c r="G1" s="8"/>
-      <c r="H1" s="9" t="s">
+      <c r="H1" s="11" t="s">
         <v>47</v>
       </c>
-      <c r="I1" s="9"/>
-      <c r="J1" s="9"/>
-      <c r="K1" s="9"/>
-      <c r="L1" s="9" t="s">
+      <c r="I1" s="11"/>
+      <c r="J1" s="11"/>
+      <c r="K1" s="11"/>
+      <c r="L1" s="11" t="s">
         <v>43</v>
       </c>
-      <c r="M1" s="9"/>
-      <c r="N1" s="9"/>
-      <c r="O1" s="9"/>
+      <c r="M1" s="11"/>
+      <c r="N1" s="11"/>
+      <c r="O1" s="11"/>
     </row>
     <row r="2" spans="1:15" x14ac:dyDescent="0.3">
-      <c r="B2" s="9" t="s">
+      <c r="B2" s="11" t="s">
         <v>38</v>
       </c>
-      <c r="C2" s="9"/>
-      <c r="D2" s="9"/>
-      <c r="E2" s="9"/>
+      <c r="C2" s="11"/>
+      <c r="D2" s="11"/>
+      <c r="E2" s="11"/>
       <c r="F2" s="8"/>
       <c r="G2" s="8"/>
       <c r="H2" s="7"/>
       <c r="I2" s="7"/>
       <c r="J2" s="7"/>
       <c r="K2" s="7"/>
-      <c r="L2" s="9" t="s">
+      <c r="L2" s="11" t="s">
         <v>42</v>
       </c>
-      <c r="M2" s="9"/>
-      <c r="N2" s="9"/>
-      <c r="O2" s="9"/>
+      <c r="M2" s="11"/>
+      <c r="N2" s="11"/>
+      <c r="O2" s="11"/>
     </row>
     <row r="3" spans="1:15" x14ac:dyDescent="0.3">
-      <c r="B3" s="9" t="s">
+      <c r="B3" s="11" t="s">
         <v>39</v>
       </c>
-      <c r="C3" s="9"/>
-      <c r="D3" s="9"/>
-      <c r="E3" s="9"/>
+      <c r="C3" s="11"/>
+      <c r="D3" s="11"/>
+      <c r="E3" s="11"/>
       <c r="F3" s="8"/>
       <c r="G3" s="8"/>
-      <c r="H3" s="9" t="s">
+      <c r="H3" s="11" t="s">
         <v>39</v>
       </c>
-      <c r="I3" s="9"/>
-      <c r="J3" s="9"/>
-      <c r="K3" s="9"/>
-      <c r="L3" s="9" t="s">
+      <c r="I3" s="11"/>
+      <c r="J3" s="11"/>
+      <c r="K3" s="11"/>
+      <c r="L3" s="11" t="s">
         <v>45</v>
       </c>
-      <c r="M3" s="9"/>
-      <c r="N3" s="9"/>
-      <c r="O3" s="9"/>
+      <c r="M3" s="11"/>
+      <c r="N3" s="11"/>
+      <c r="O3" s="11"/>
     </row>
     <row r="4" spans="1:15" x14ac:dyDescent="0.3">
-      <c r="B4" s="9" t="s">
+      <c r="B4" s="11" t="s">
         <v>41</v>
       </c>
-      <c r="C4" s="9"/>
-      <c r="D4" s="9" t="s">
+      <c r="C4" s="11"/>
+      <c r="D4" s="11" t="s">
         <v>40</v>
       </c>
-      <c r="E4" s="9"/>
+      <c r="E4" s="11"/>
       <c r="F4" s="8"/>
       <c r="G4" s="8"/>
-      <c r="H4" s="9" t="s">
+      <c r="H4" s="11" t="s">
         <v>41</v>
       </c>
-      <c r="I4" s="9"/>
-      <c r="J4" s="9" t="s">
+      <c r="I4" s="11"/>
+      <c r="J4" s="11" t="s">
         <v>40</v>
       </c>
-      <c r="K4" s="9"/>
+      <c r="K4" s="11"/>
     </row>
     <row r="5" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A5" t="s">
@@ -1645,88 +1693,88 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:15" x14ac:dyDescent="0.3">
-      <c r="B1" s="9" t="s">
+      <c r="B1" s="11" t="s">
         <v>44</v>
       </c>
-      <c r="C1" s="9"/>
-      <c r="D1" s="9"/>
-      <c r="E1" s="9"/>
+      <c r="C1" s="11"/>
+      <c r="D1" s="11"/>
+      <c r="E1" s="11"/>
       <c r="F1" s="8"/>
       <c r="G1" s="8"/>
-      <c r="H1" s="9" t="s">
+      <c r="H1" s="11" t="s">
         <v>47</v>
       </c>
-      <c r="I1" s="9"/>
-      <c r="J1" s="9"/>
-      <c r="K1" s="9"/>
-      <c r="L1" s="9" t="s">
+      <c r="I1" s="11"/>
+      <c r="J1" s="11"/>
+      <c r="K1" s="11"/>
+      <c r="L1" s="11" t="s">
         <v>43</v>
       </c>
-      <c r="M1" s="9"/>
-      <c r="N1" s="9"/>
-      <c r="O1" s="9"/>
+      <c r="M1" s="11"/>
+      <c r="N1" s="11"/>
+      <c r="O1" s="11"/>
     </row>
     <row r="2" spans="1:15" x14ac:dyDescent="0.3">
-      <c r="B2" s="9" t="s">
+      <c r="B2" s="11" t="s">
         <v>38</v>
       </c>
-      <c r="C2" s="9"/>
-      <c r="D2" s="9"/>
-      <c r="E2" s="9"/>
+      <c r="C2" s="11"/>
+      <c r="D2" s="11"/>
+      <c r="E2" s="11"/>
       <c r="F2" s="8"/>
       <c r="G2" s="8"/>
       <c r="H2" s="7"/>
       <c r="I2" s="7"/>
       <c r="J2" s="7"/>
       <c r="K2" s="7"/>
-      <c r="L2" s="9" t="s">
+      <c r="L2" s="11" t="s">
         <v>42</v>
       </c>
-      <c r="M2" s="9"/>
-      <c r="N2" s="9"/>
-      <c r="O2" s="9"/>
+      <c r="M2" s="11"/>
+      <c r="N2" s="11"/>
+      <c r="O2" s="11"/>
     </row>
     <row r="3" spans="1:15" x14ac:dyDescent="0.3">
-      <c r="B3" s="9" t="s">
+      <c r="B3" s="11" t="s">
         <v>39</v>
       </c>
-      <c r="C3" s="9"/>
-      <c r="D3" s="9"/>
-      <c r="E3" s="9"/>
+      <c r="C3" s="11"/>
+      <c r="D3" s="11"/>
+      <c r="E3" s="11"/>
       <c r="F3" s="8"/>
       <c r="G3" s="8"/>
-      <c r="H3" s="9" t="s">
+      <c r="H3" s="11" t="s">
         <v>39</v>
       </c>
-      <c r="I3" s="9"/>
-      <c r="J3" s="9"/>
-      <c r="K3" s="9"/>
-      <c r="L3" s="9" t="s">
+      <c r="I3" s="11"/>
+      <c r="J3" s="11"/>
+      <c r="K3" s="11"/>
+      <c r="L3" s="11" t="s">
         <v>45</v>
       </c>
-      <c r="M3" s="9"/>
-      <c r="N3" s="9"/>
-      <c r="O3" s="9"/>
+      <c r="M3" s="11"/>
+      <c r="N3" s="11"/>
+      <c r="O3" s="11"/>
     </row>
     <row r="4" spans="1:15" x14ac:dyDescent="0.3">
-      <c r="B4" s="9" t="s">
+      <c r="B4" s="11" t="s">
         <v>41</v>
       </c>
-      <c r="C4" s="9"/>
-      <c r="D4" s="9" t="s">
+      <c r="C4" s="11"/>
+      <c r="D4" s="11" t="s">
         <v>40</v>
       </c>
-      <c r="E4" s="9"/>
+      <c r="E4" s="11"/>
       <c r="F4" s="8"/>
       <c r="G4" s="8"/>
-      <c r="H4" s="9" t="s">
+      <c r="H4" s="11" t="s">
         <v>41</v>
       </c>
-      <c r="I4" s="9"/>
-      <c r="J4" s="9" t="s">
+      <c r="I4" s="11"/>
+      <c r="J4" s="11" t="s">
         <v>40</v>
       </c>
-      <c r="K4" s="9"/>
+      <c r="K4" s="11"/>
     </row>
     <row r="5" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A5" t="s">
@@ -2441,377 +2489,2456 @@
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:C34"/>
+  <dimension ref="A1:C36"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="B1" sqref="B1:C16"/>
+      <selection activeCell="B21" sqref="B21:C36"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <sheetData>
     <row r="1" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A1" t="s">
-        <v>19</v>
-      </c>
-      <c r="B1">
-        <v>2230.1799999999998</v>
-      </c>
-      <c r="C1">
-        <v>51.69</v>
+        <v>54</v>
       </c>
     </row>
     <row r="2" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A2" t="s">
-        <v>20</v>
-      </c>
-      <c r="B2">
-        <v>1038.1400000000001</v>
-      </c>
-      <c r="C2">
-        <v>38.46</v>
+        <v>53</v>
       </c>
     </row>
     <row r="3" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A3" t="s">
-        <v>21</v>
+        <v>19</v>
       </c>
       <c r="B3">
-        <v>2194.4899999999998</v>
+        <v>1900.63</v>
       </c>
       <c r="C3">
-        <v>24.45</v>
+        <v>2.7490000000000001</v>
       </c>
     </row>
     <row r="4" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A4" t="s">
-        <v>22</v>
+        <v>20</v>
       </c>
       <c r="B4">
-        <v>984.37199999999996</v>
+        <v>870.03599999999994</v>
       </c>
       <c r="C4">
-        <v>6.0309999999999997</v>
+        <v>3.5089999999999999</v>
       </c>
     </row>
     <row r="5" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A5" t="s">
-        <v>23</v>
+        <v>21</v>
       </c>
       <c r="B5">
-        <v>2664.36</v>
+        <v>1712.46</v>
       </c>
       <c r="C5">
-        <v>29.64</v>
+        <v>0.58979999999999999</v>
       </c>
     </row>
     <row r="6" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A6" t="s">
-        <v>24</v>
+        <v>22</v>
       </c>
       <c r="B6">
-        <v>1349.47</v>
+        <v>760.15700000000004</v>
       </c>
       <c r="C6">
-        <v>26.73</v>
+        <v>0.76529999999999998</v>
       </c>
     </row>
     <row r="7" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A7" t="s">
-        <v>25</v>
+        <v>23</v>
       </c>
       <c r="B7">
-        <v>2527.86</v>
+        <v>2450.8200000000002</v>
       </c>
       <c r="C7">
-        <v>16.739999999999998</v>
+        <v>4.8659999999999997</v>
       </c>
     </row>
     <row r="8" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A8" t="s">
-        <v>26</v>
+        <v>24</v>
       </c>
       <c r="B8">
-        <v>1300.98</v>
+        <v>1319.29</v>
       </c>
       <c r="C8">
-        <v>44.04</v>
+        <v>3.4140000000000001</v>
       </c>
     </row>
     <row r="9" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A9" t="s">
-        <v>27</v>
+        <v>25</v>
       </c>
       <c r="B9">
-        <v>1567.46</v>
+        <v>1887.36</v>
       </c>
       <c r="C9">
-        <v>11.79</v>
+        <v>1.452</v>
       </c>
     </row>
     <row r="10" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A10" t="s">
-        <v>28</v>
+        <v>26</v>
       </c>
       <c r="B10">
-        <v>415.22699999999998</v>
+        <v>890.28200000000004</v>
       </c>
       <c r="C10">
-        <v>27.26</v>
+        <v>2.5430000000000001</v>
       </c>
     </row>
     <row r="11" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A11" t="s">
-        <v>29</v>
+        <v>27</v>
       </c>
       <c r="B11">
-        <v>2654.8</v>
+        <v>1510.5</v>
       </c>
       <c r="C11">
-        <v>52.39</v>
+        <v>4.867</v>
       </c>
     </row>
     <row r="12" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A12" t="s">
-        <v>30</v>
+        <v>28</v>
       </c>
       <c r="B12">
-        <v>1053.0899999999999</v>
+        <v>237.07</v>
       </c>
       <c r="C12">
-        <v>17.62</v>
+        <v>0.39090000000000003</v>
       </c>
     </row>
     <row r="13" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A13" t="s">
-        <v>31</v>
+        <v>29</v>
       </c>
       <c r="B13">
-        <v>2511.9299999999998</v>
+        <v>2285.96</v>
       </c>
       <c r="C13">
-        <v>60.8</v>
+        <v>11.44</v>
       </c>
     </row>
     <row r="14" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A14" t="s">
-        <v>32</v>
+        <v>30</v>
       </c>
       <c r="B14">
-        <v>1021.93</v>
+        <v>619.279</v>
       </c>
       <c r="C14">
-        <v>6.0380000000000003</v>
+        <v>3.2890000000000001</v>
       </c>
     </row>
     <row r="15" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A15" t="s">
-        <v>33</v>
+        <v>31</v>
       </c>
       <c r="B15">
-        <v>3781.97</v>
+        <v>2115.15</v>
       </c>
       <c r="C15">
-        <v>34.090000000000003</v>
+        <v>0.75600000000000001</v>
       </c>
     </row>
     <row r="16" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A16" t="s">
-        <v>34</v>
+        <v>32</v>
       </c>
       <c r="B16">
-        <v>3850.59</v>
+        <v>542.00300000000004</v>
       </c>
       <c r="C16">
-        <v>23.89</v>
+        <v>0.77070000000000005</v>
       </c>
     </row>
     <row r="17" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A17" t="s">
-        <v>48</v>
+        <v>33</v>
+      </c>
+      <c r="B17">
+        <v>3547.4</v>
+      </c>
+      <c r="C17">
+        <v>8.2409999999999997</v>
       </c>
     </row>
     <row r="18" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A18" t="s">
-        <v>49</v>
+        <v>34</v>
+      </c>
+      <c r="B18">
+        <v>3512.47</v>
+      </c>
+      <c r="C18">
+        <v>5.4960000000000004</v>
       </c>
     </row>
     <row r="19" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A19" t="s">
-        <v>19</v>
-      </c>
-      <c r="B19">
-        <v>1807.61</v>
-      </c>
-      <c r="C19">
-        <v>14.77</v>
+        <v>48</v>
       </c>
     </row>
     <row r="20" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A20" t="s">
-        <v>20</v>
-      </c>
-      <c r="B20">
-        <v>1080.57</v>
-      </c>
-      <c r="C20">
-        <v>28.56</v>
+        <v>53</v>
       </c>
     </row>
     <row r="21" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A21" t="s">
-        <v>21</v>
+        <v>19</v>
       </c>
       <c r="B21">
-        <v>1850.37</v>
+        <v>1399.54</v>
       </c>
       <c r="C21">
-        <v>26.47</v>
+        <v>10.9</v>
       </c>
     </row>
     <row r="22" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A22" t="s">
-        <v>22</v>
+        <v>20</v>
       </c>
       <c r="B22">
-        <v>986.70699999999999</v>
+        <v>302.964</v>
       </c>
       <c r="C22">
-        <v>6.2270000000000003</v>
+        <v>10.55</v>
       </c>
     </row>
     <row r="23" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A23" t="s">
-        <v>23</v>
+        <v>21</v>
       </c>
       <c r="B23">
-        <v>1384.33</v>
+        <v>1313.2</v>
       </c>
       <c r="C23">
-        <v>27.78</v>
+        <v>1.407</v>
       </c>
     </row>
     <row r="24" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A24" t="s">
-        <v>24</v>
+        <v>22</v>
       </c>
       <c r="B24">
-        <v>554.97299999999996</v>
+        <v>300.86099999999999</v>
       </c>
       <c r="C24">
-        <v>4.5730000000000004</v>
+        <v>4.7169999999999996</v>
       </c>
     </row>
     <row r="25" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A25" t="s">
-        <v>25</v>
+        <v>23</v>
       </c>
       <c r="B25">
-        <v>1385.12</v>
+        <v>1129.69</v>
       </c>
       <c r="C25">
-        <v>8.7919999999999998</v>
+        <v>7.4560000000000004</v>
       </c>
     </row>
     <row r="26" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A26" t="s">
-        <v>26</v>
+        <v>24</v>
       </c>
       <c r="B26">
-        <v>624.61500000000001</v>
+        <v>294.54599999999999</v>
       </c>
       <c r="C26">
-        <v>3.4</v>
+        <v>2.4689999999999999</v>
       </c>
     </row>
     <row r="27" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A27" t="s">
-        <v>27</v>
+        <v>25</v>
       </c>
       <c r="B27">
-        <v>1122.28</v>
+        <v>1149.96</v>
       </c>
       <c r="C27">
-        <v>3.2120000000000002</v>
+        <v>1.603</v>
       </c>
     </row>
     <row r="28" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A28" t="s">
-        <v>28</v>
+        <v>26</v>
       </c>
       <c r="B28">
-        <v>311.81900000000002</v>
+        <v>306.721</v>
       </c>
       <c r="C28">
-        <v>18.72</v>
+        <v>1.768</v>
       </c>
     </row>
     <row r="29" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A29" t="s">
-        <v>29</v>
+        <v>27</v>
       </c>
       <c r="B29">
-        <v>1313.08</v>
+        <v>1076.6099999999999</v>
       </c>
       <c r="C29">
-        <v>3.2519999999999998</v>
+        <v>0.5413</v>
       </c>
     </row>
     <row r="30" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A30" t="s">
-        <v>30</v>
+        <v>28</v>
       </c>
       <c r="B30">
-        <v>465.65699999999998</v>
+        <v>134.37799999999999</v>
       </c>
       <c r="C30">
-        <v>4.0910000000000002</v>
+        <v>0.6633</v>
       </c>
     </row>
     <row r="31" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A31" t="s">
-        <v>31</v>
+        <v>29</v>
       </c>
       <c r="B31">
-        <v>1310.05</v>
+        <v>1269.44</v>
       </c>
       <c r="C31">
-        <v>8.125</v>
+        <v>6.3460000000000001</v>
       </c>
     </row>
     <row r="32" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A32" t="s">
-        <v>32</v>
+        <v>30</v>
       </c>
       <c r="B32">
-        <v>470.31400000000002</v>
+        <v>170.28800000000001</v>
       </c>
       <c r="C32">
-        <v>0.9476</v>
+        <v>0.34689999999999999</v>
       </c>
     </row>
     <row r="33" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A33" t="s">
-        <v>33</v>
+        <v>31</v>
       </c>
       <c r="B33">
-        <v>499.59100000000001</v>
+        <v>1297.02</v>
       </c>
       <c r="C33">
-        <v>2.3250000000000002</v>
+        <v>3.21</v>
       </c>
     </row>
     <row r="34" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A34" t="s">
+        <v>32</v>
+      </c>
+      <c r="B34">
+        <v>173.244</v>
+      </c>
+      <c r="C34">
+        <v>0.52170000000000005</v>
+      </c>
+    </row>
+    <row r="35" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A35" t="s">
+        <v>33</v>
+      </c>
+      <c r="B35">
+        <v>191.03299999999999</v>
+      </c>
+      <c r="C35">
+        <v>1.016</v>
+      </c>
+    </row>
+    <row r="36" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A36" t="s">
         <v>34</v>
       </c>
-      <c r="B34">
-        <v>484.92899999999997</v>
-      </c>
-      <c r="C34">
-        <v>2.6859999999999999</v>
+      <c r="B36">
+        <v>232.67099999999999</v>
+      </c>
+      <c r="C36">
+        <v>5.0629999999999997</v>
       </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:U22"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="H10" sqref="H10"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <cols>
+    <col min="1" max="1" width="80.88671875" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="14.109375" customWidth="1"/>
+    <col min="3" max="3" width="8.77734375" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="14.77734375" customWidth="1"/>
+    <col min="6" max="6" width="13.5546875" customWidth="1"/>
+    <col min="8" max="8" width="13.77734375" customWidth="1"/>
+    <col min="9" max="9" width="9.109375" customWidth="1"/>
+    <col min="14" max="14" width="14.77734375" customWidth="1"/>
+    <col min="16" max="16" width="12.77734375" customWidth="1"/>
+    <col min="18" max="18" width="22.109375" customWidth="1"/>
+    <col min="19" max="19" width="12.88671875" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:21" x14ac:dyDescent="0.3">
+      <c r="B1" s="11" t="s">
+        <v>44</v>
+      </c>
+      <c r="C1" s="11"/>
+      <c r="D1" s="11"/>
+      <c r="E1" s="11"/>
+      <c r="F1" s="11"/>
+      <c r="G1" s="11"/>
+      <c r="H1" s="11"/>
+      <c r="I1" s="11"/>
+      <c r="J1" s="11"/>
+      <c r="K1" s="11"/>
+      <c r="L1" s="11"/>
+      <c r="M1" s="11"/>
+      <c r="N1" s="11" t="s">
+        <v>47</v>
+      </c>
+      <c r="O1" s="11"/>
+      <c r="P1" s="11"/>
+      <c r="Q1" s="11"/>
+      <c r="R1" s="11" t="s">
+        <v>43</v>
+      </c>
+      <c r="S1" s="11"/>
+      <c r="T1" s="11"/>
+      <c r="U1" s="11"/>
+    </row>
+    <row r="2" spans="1:21" x14ac:dyDescent="0.3">
+      <c r="B2" s="11" t="s">
+        <v>38</v>
+      </c>
+      <c r="C2" s="11"/>
+      <c r="D2" s="11"/>
+      <c r="E2" s="11"/>
+      <c r="F2" s="11"/>
+      <c r="G2" s="11"/>
+      <c r="H2" s="11"/>
+      <c r="I2" s="11"/>
+      <c r="J2" s="11"/>
+      <c r="K2" s="11"/>
+      <c r="L2" s="11"/>
+      <c r="M2" s="11"/>
+      <c r="N2" s="9"/>
+      <c r="O2" s="9"/>
+      <c r="P2" s="9"/>
+      <c r="Q2" s="9"/>
+      <c r="R2" s="11" t="s">
+        <v>42</v>
+      </c>
+      <c r="S2" s="11"/>
+      <c r="T2" s="11"/>
+      <c r="U2" s="11"/>
+    </row>
+    <row r="3" spans="1:21" x14ac:dyDescent="0.3">
+      <c r="B3" s="11" t="s">
+        <v>39</v>
+      </c>
+      <c r="C3" s="11"/>
+      <c r="D3" s="11"/>
+      <c r="E3" s="11"/>
+      <c r="F3" s="11"/>
+      <c r="G3" s="11"/>
+      <c r="H3" s="11"/>
+      <c r="I3" s="11"/>
+      <c r="J3" s="11"/>
+      <c r="K3" s="11"/>
+      <c r="L3" s="11"/>
+      <c r="M3" s="11"/>
+      <c r="N3" s="11" t="s">
+        <v>39</v>
+      </c>
+      <c r="O3" s="11"/>
+      <c r="P3" s="11"/>
+      <c r="Q3" s="11"/>
+      <c r="R3" s="11" t="s">
+        <v>45</v>
+      </c>
+      <c r="S3" s="11"/>
+      <c r="T3" s="11"/>
+      <c r="U3" s="11"/>
+    </row>
+    <row r="4" spans="1:21" x14ac:dyDescent="0.3">
+      <c r="B4" s="9"/>
+      <c r="C4" s="9"/>
+      <c r="D4" s="9"/>
+      <c r="E4" s="9"/>
+      <c r="F4" s="11" t="s">
+        <v>51</v>
+      </c>
+      <c r="G4" s="11"/>
+      <c r="H4" s="11"/>
+      <c r="I4" s="11"/>
+      <c r="J4" s="11" t="s">
+        <v>52</v>
+      </c>
+      <c r="K4" s="11"/>
+      <c r="L4" s="11"/>
+      <c r="M4" s="11"/>
+      <c r="N4" s="9"/>
+      <c r="O4" s="9"/>
+      <c r="P4" s="9"/>
+      <c r="Q4" s="9"/>
+      <c r="R4" s="9"/>
+      <c r="S4" s="9"/>
+      <c r="T4" s="9"/>
+      <c r="U4" s="9"/>
+    </row>
+    <row r="5" spans="1:21" x14ac:dyDescent="0.3">
+      <c r="B5" s="11" t="s">
+        <v>41</v>
+      </c>
+      <c r="C5" s="11"/>
+      <c r="D5" s="11" t="s">
+        <v>40</v>
+      </c>
+      <c r="E5" s="11"/>
+      <c r="F5" s="11" t="s">
+        <v>41</v>
+      </c>
+      <c r="G5" s="11"/>
+      <c r="H5" s="11" t="s">
+        <v>40</v>
+      </c>
+      <c r="I5" s="11"/>
+      <c r="J5" s="11" t="s">
+        <v>41</v>
+      </c>
+      <c r="K5" s="11"/>
+      <c r="L5" s="11" t="s">
+        <v>40</v>
+      </c>
+      <c r="M5" s="11"/>
+      <c r="N5" s="11" t="s">
+        <v>41</v>
+      </c>
+      <c r="O5" s="11"/>
+      <c r="P5" s="11" t="s">
+        <v>40</v>
+      </c>
+      <c r="Q5" s="11"/>
+    </row>
+    <row r="6" spans="1:21" x14ac:dyDescent="0.3">
+      <c r="A6" t="s">
+        <v>35</v>
+      </c>
+      <c r="B6" s="9" t="s">
+        <v>49</v>
+      </c>
+      <c r="C6" s="9" t="s">
+        <v>50</v>
+      </c>
+      <c r="D6" s="9" t="s">
+        <v>49</v>
+      </c>
+      <c r="E6" s="9" t="s">
+        <v>50</v>
+      </c>
+      <c r="F6" s="9" t="s">
+        <v>49</v>
+      </c>
+      <c r="G6" s="9" t="s">
+        <v>50</v>
+      </c>
+      <c r="H6" s="9" t="s">
+        <v>49</v>
+      </c>
+      <c r="I6" s="9" t="s">
+        <v>50</v>
+      </c>
+      <c r="J6" s="9" t="s">
+        <v>49</v>
+      </c>
+      <c r="K6" s="9" t="s">
+        <v>50</v>
+      </c>
+      <c r="L6" s="9" t="s">
+        <v>49</v>
+      </c>
+      <c r="M6" s="9" t="s">
+        <v>50</v>
+      </c>
+      <c r="N6" t="s">
+        <v>36</v>
+      </c>
+      <c r="O6" t="s">
+        <v>37</v>
+      </c>
+      <c r="P6" t="s">
+        <v>36</v>
+      </c>
+      <c r="Q6" t="s">
+        <v>37</v>
+      </c>
+      <c r="R6" t="s">
+        <v>36</v>
+      </c>
+      <c r="S6" t="s">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="7" spans="1:21" x14ac:dyDescent="0.3">
+      <c r="A7" t="s">
+        <v>19</v>
+      </c>
+      <c r="B7" s="6">
+        <v>2325.48</v>
+      </c>
+      <c r="C7" s="6">
+        <v>108.1</v>
+      </c>
+      <c r="D7" s="6">
+        <v>2465.0100000000002</v>
+      </c>
+      <c r="E7" s="6">
+        <v>166</v>
+      </c>
+      <c r="F7" s="6">
+        <v>2291.04</v>
+      </c>
+      <c r="G7" s="6">
+        <v>71.03</v>
+      </c>
+      <c r="H7" s="6">
+        <v>2361.7600000000002</v>
+      </c>
+      <c r="I7" s="6">
+        <v>71.75</v>
+      </c>
+      <c r="J7" s="6">
+        <v>2315.4299999999998</v>
+      </c>
+      <c r="K7" s="6">
+        <v>78.13</v>
+      </c>
+      <c r="L7" s="6">
+        <v>2413.85</v>
+      </c>
+      <c r="M7" s="6">
+        <v>82.58</v>
+      </c>
+      <c r="N7" s="6"/>
+      <c r="O7" s="6"/>
+      <c r="P7" s="6"/>
+      <c r="Q7" s="6"/>
+      <c r="R7" s="6">
+        <v>1900.63</v>
+      </c>
+      <c r="S7" s="6">
+        <v>2.7490000000000001</v>
+      </c>
+    </row>
+    <row r="8" spans="1:21" x14ac:dyDescent="0.3">
+      <c r="A8" t="s">
+        <v>20</v>
+      </c>
+      <c r="B8" s="6">
+        <v>1057.78</v>
+      </c>
+      <c r="C8" s="6">
+        <v>19.47</v>
+      </c>
+      <c r="D8" s="6">
+        <v>1107.4000000000001</v>
+      </c>
+      <c r="E8" s="6">
+        <v>55.46</v>
+      </c>
+      <c r="F8" s="6">
+        <v>936.12099999999998</v>
+      </c>
+      <c r="G8" s="6">
+        <v>6.1040000000000001</v>
+      </c>
+      <c r="H8" s="6">
+        <v>818.85</v>
+      </c>
+      <c r="I8" s="6">
+        <v>7.7190000000000003</v>
+      </c>
+      <c r="J8" s="6">
+        <v>940.49599999999998</v>
+      </c>
+      <c r="K8" s="6">
+        <v>4.8280000000000003</v>
+      </c>
+      <c r="L8" s="6">
+        <v>878.05600000000004</v>
+      </c>
+      <c r="M8" s="6">
+        <v>141.9</v>
+      </c>
+      <c r="N8" s="6"/>
+      <c r="O8" s="6"/>
+      <c r="P8" s="6"/>
+      <c r="Q8" s="6"/>
+      <c r="R8" s="6">
+        <v>870.03599999999994</v>
+      </c>
+      <c r="S8" s="6">
+        <v>3.5089999999999999</v>
+      </c>
+    </row>
+    <row r="9" spans="1:21" x14ac:dyDescent="0.3">
+      <c r="A9" t="s">
+        <v>21</v>
+      </c>
+      <c r="B9" s="6">
+        <v>2203.9299999999998</v>
+      </c>
+      <c r="C9" s="6">
+        <v>41.18</v>
+      </c>
+      <c r="D9" s="6">
+        <v>2402.94</v>
+      </c>
+      <c r="E9" s="6">
+        <v>106.5</v>
+      </c>
+      <c r="F9" s="6">
+        <v>2200.9699999999998</v>
+      </c>
+      <c r="G9" s="6">
+        <v>15.25</v>
+      </c>
+      <c r="H9" s="6">
+        <v>2187.73</v>
+      </c>
+      <c r="I9" s="6">
+        <v>11.19</v>
+      </c>
+      <c r="J9" s="6">
+        <v>2208.1</v>
+      </c>
+      <c r="K9" s="6">
+        <v>27.92</v>
+      </c>
+      <c r="L9" s="6">
+        <v>2199.91</v>
+      </c>
+      <c r="M9" s="6">
+        <v>28.09</v>
+      </c>
+      <c r="N9" s="6"/>
+      <c r="O9" s="6"/>
+      <c r="P9" s="6"/>
+      <c r="Q9" s="6"/>
+      <c r="R9" s="6">
+        <v>1712.46</v>
+      </c>
+      <c r="S9" s="6">
+        <v>0.58979999999999999</v>
+      </c>
+    </row>
+    <row r="10" spans="1:21" x14ac:dyDescent="0.3">
+      <c r="A10" t="s">
+        <v>22</v>
+      </c>
+      <c r="B10" s="6">
+        <v>1033.07</v>
+      </c>
+      <c r="C10" s="6">
+        <v>8.0640000000000001</v>
+      </c>
+      <c r="D10" s="6">
+        <v>1136.49</v>
+      </c>
+      <c r="E10" s="6">
+        <v>148.6</v>
+      </c>
+      <c r="F10" s="6">
+        <v>930.18499999999995</v>
+      </c>
+      <c r="G10" s="6">
+        <v>8.6579999999999995</v>
+      </c>
+      <c r="H10" s="6">
+        <v>778.59100000000001</v>
+      </c>
+      <c r="I10" s="6">
+        <v>21.75</v>
+      </c>
+      <c r="J10" s="6">
+        <v>936.54100000000005</v>
+      </c>
+      <c r="K10" s="6">
+        <v>24.01</v>
+      </c>
+      <c r="L10" s="6">
+        <v>775.92100000000005</v>
+      </c>
+      <c r="M10" s="6">
+        <v>6.8449999999999998</v>
+      </c>
+      <c r="N10" s="6"/>
+      <c r="O10" s="6"/>
+      <c r="P10" s="6"/>
+      <c r="Q10" s="6"/>
+      <c r="R10" s="6">
+        <v>760.15700000000004</v>
+      </c>
+      <c r="S10" s="6">
+        <v>0.76529999999999998</v>
+      </c>
+    </row>
+    <row r="11" spans="1:21" x14ac:dyDescent="0.3">
+      <c r="A11" t="s">
+        <v>23</v>
+      </c>
+      <c r="B11" s="6">
+        <v>2672.72</v>
+      </c>
+      <c r="C11" s="6">
+        <v>30.49</v>
+      </c>
+      <c r="D11" s="6">
+        <v>3037.59</v>
+      </c>
+      <c r="E11" s="6">
+        <v>237.3</v>
+      </c>
+      <c r="F11" s="6">
+        <v>2752.01</v>
+      </c>
+      <c r="G11" s="6">
+        <v>49.76</v>
+      </c>
+      <c r="H11" s="6">
+        <v>2629.91</v>
+      </c>
+      <c r="I11" s="6">
+        <v>13.95</v>
+      </c>
+      <c r="J11" s="6">
+        <v>2723.93</v>
+      </c>
+      <c r="K11" s="6">
+        <v>46.87</v>
+      </c>
+      <c r="L11" s="6">
+        <v>2672.79</v>
+      </c>
+      <c r="M11" s="6">
+        <v>30.29</v>
+      </c>
+      <c r="N11" s="6"/>
+      <c r="O11" s="6"/>
+      <c r="P11" s="6"/>
+      <c r="Q11" s="6"/>
+      <c r="R11" s="6">
+        <v>2450.8200000000002</v>
+      </c>
+      <c r="S11" s="6">
+        <v>4.8659999999999997</v>
+      </c>
+    </row>
+    <row r="12" spans="1:21" x14ac:dyDescent="0.3">
+      <c r="A12" t="s">
+        <v>24</v>
+      </c>
+      <c r="B12" s="6">
+        <v>1436.33</v>
+      </c>
+      <c r="C12" s="6">
+        <v>20.51</v>
+      </c>
+      <c r="D12" s="6">
+        <v>1491.05</v>
+      </c>
+      <c r="E12" s="6">
+        <v>145.69999999999999</v>
+      </c>
+      <c r="F12" s="6">
+        <v>1381.16</v>
+      </c>
+      <c r="G12" s="6">
+        <v>7.2880000000000003</v>
+      </c>
+      <c r="H12" s="6">
+        <v>1164.21</v>
+      </c>
+      <c r="I12" s="6">
+        <v>8.8089999999999993</v>
+      </c>
+      <c r="J12" s="6">
+        <v>1393.16</v>
+      </c>
+      <c r="K12" s="6">
+        <v>31.7</v>
+      </c>
+      <c r="L12" s="6">
+        <v>1209.81</v>
+      </c>
+      <c r="M12" s="6">
+        <v>70.13</v>
+      </c>
+      <c r="N12" s="6"/>
+      <c r="O12" s="6"/>
+      <c r="P12" s="6"/>
+      <c r="Q12" s="6"/>
+      <c r="R12" s="6">
+        <v>1319.29</v>
+      </c>
+      <c r="S12" s="6">
+        <v>3.4140000000000001</v>
+      </c>
+    </row>
+    <row r="13" spans="1:21" x14ac:dyDescent="0.3">
+      <c r="A13" t="s">
+        <v>25</v>
+      </c>
+      <c r="B13" s="6">
+        <v>2617.0100000000002</v>
+      </c>
+      <c r="C13" s="6">
+        <v>13.95</v>
+      </c>
+      <c r="D13" s="6">
+        <v>2822.02</v>
+      </c>
+      <c r="E13" s="6">
+        <v>184.8</v>
+      </c>
+      <c r="F13" s="6">
+        <v>2638.54</v>
+      </c>
+      <c r="G13" s="6">
+        <v>14.31</v>
+      </c>
+      <c r="H13" s="6">
+        <v>2591.98</v>
+      </c>
+      <c r="I13" s="6">
+        <v>46.59</v>
+      </c>
+      <c r="J13" s="6">
+        <v>2607.9</v>
+      </c>
+      <c r="K13" s="6">
+        <v>21.54</v>
+      </c>
+      <c r="L13" s="6">
+        <v>2597.59</v>
+      </c>
+      <c r="M13" s="6">
+        <v>25.98</v>
+      </c>
+      <c r="N13" s="6"/>
+      <c r="O13" s="6"/>
+      <c r="P13" s="6"/>
+      <c r="Q13" s="6"/>
+      <c r="R13" s="6">
+        <v>1887.36</v>
+      </c>
+      <c r="S13" s="6">
+        <v>1.452</v>
+      </c>
+    </row>
+    <row r="14" spans="1:21" x14ac:dyDescent="0.3">
+      <c r="A14" t="s">
+        <v>26</v>
+      </c>
+      <c r="B14" s="6">
+        <v>1438.28</v>
+      </c>
+      <c r="C14" s="6">
+        <v>44.19</v>
+      </c>
+      <c r="D14" s="6">
+        <v>1442.59</v>
+      </c>
+      <c r="E14" s="6">
+        <v>142.30000000000001</v>
+      </c>
+      <c r="F14" s="6">
+        <v>1365.28</v>
+      </c>
+      <c r="G14" s="6">
+        <v>33.4</v>
+      </c>
+      <c r="H14" s="6">
+        <v>1127.51</v>
+      </c>
+      <c r="I14" s="6">
+        <v>7.7030000000000003</v>
+      </c>
+      <c r="J14" s="6">
+        <v>1345.64</v>
+      </c>
+      <c r="K14" s="6">
+        <v>8.7919999999999998</v>
+      </c>
+      <c r="L14" s="6">
+        <v>1135.51</v>
+      </c>
+      <c r="M14" s="6">
+        <v>9.5150000000000006</v>
+      </c>
+      <c r="N14" s="6"/>
+      <c r="O14" s="6"/>
+      <c r="P14" s="6"/>
+      <c r="Q14" s="6"/>
+      <c r="R14" s="6">
+        <v>890.28200000000004</v>
+      </c>
+      <c r="S14" s="6">
+        <v>2.5430000000000001</v>
+      </c>
+    </row>
+    <row r="15" spans="1:21" x14ac:dyDescent="0.3">
+      <c r="A15" t="s">
+        <v>27</v>
+      </c>
+      <c r="B15" s="6">
+        <v>1657.63</v>
+      </c>
+      <c r="C15" s="6">
+        <v>9.782</v>
+      </c>
+      <c r="D15" s="6">
+        <v>1754.92</v>
+      </c>
+      <c r="E15" s="6">
+        <v>182.8</v>
+      </c>
+      <c r="F15" s="6">
+        <v>1665.68</v>
+      </c>
+      <c r="G15" s="6">
+        <v>13.22</v>
+      </c>
+      <c r="H15" s="6">
+        <v>1593.35</v>
+      </c>
+      <c r="I15" s="6">
+        <v>42.78</v>
+      </c>
+      <c r="J15" s="6">
+        <v>1660.91</v>
+      </c>
+      <c r="K15" s="6">
+        <v>17</v>
+      </c>
+      <c r="L15" s="6">
+        <v>1584.22</v>
+      </c>
+      <c r="M15" s="6">
+        <v>13.02</v>
+      </c>
+      <c r="N15" s="6"/>
+      <c r="O15" s="6"/>
+      <c r="P15" s="6"/>
+      <c r="Q15" s="6"/>
+      <c r="R15" s="6">
+        <v>1510.5</v>
+      </c>
+      <c r="S15" s="6">
+        <v>4.867</v>
+      </c>
+    </row>
+    <row r="16" spans="1:21" x14ac:dyDescent="0.3">
+      <c r="A16" t="s">
+        <v>28</v>
+      </c>
+      <c r="B16" s="6">
+        <v>529.57100000000003</v>
+      </c>
+      <c r="C16" s="6">
+        <v>2.4169999999999998</v>
+      </c>
+      <c r="D16" s="6">
+        <v>433.5</v>
+      </c>
+      <c r="E16" s="6">
+        <v>25.27</v>
+      </c>
+      <c r="F16" s="6">
+        <v>520.19299999999998</v>
+      </c>
+      <c r="G16" s="6">
+        <v>3.9289999999999998</v>
+      </c>
+      <c r="H16" s="6">
+        <v>404.46499999999997</v>
+      </c>
+      <c r="I16" s="6">
+        <v>1.9259999999999999</v>
+      </c>
+      <c r="J16" s="6">
+        <v>523.84400000000005</v>
+      </c>
+      <c r="K16" s="6">
+        <v>3.714</v>
+      </c>
+      <c r="L16" s="6">
+        <v>407.39</v>
+      </c>
+      <c r="M16" s="6">
+        <v>5.3140000000000001</v>
+      </c>
+      <c r="N16" s="6"/>
+      <c r="O16" s="6"/>
+      <c r="P16" s="6"/>
+      <c r="Q16" s="6"/>
+      <c r="R16" s="6">
+        <v>237.07</v>
+      </c>
+      <c r="S16" s="6">
+        <v>0.39090000000000003</v>
+      </c>
+    </row>
+    <row r="17" spans="1:19" x14ac:dyDescent="0.3">
+      <c r="A17" t="s">
+        <v>29</v>
+      </c>
+      <c r="B17" s="6">
+        <v>2953.78</v>
+      </c>
+      <c r="C17" s="6">
+        <v>162.19999999999999</v>
+      </c>
+      <c r="D17" s="6">
+        <v>2916.86</v>
+      </c>
+      <c r="E17" s="6">
+        <v>168.4</v>
+      </c>
+      <c r="F17" s="6">
+        <v>2943.07</v>
+      </c>
+      <c r="G17" s="6">
+        <v>198</v>
+      </c>
+      <c r="H17" s="6">
+        <v>2652.9</v>
+      </c>
+      <c r="I17" s="6">
+        <v>105</v>
+      </c>
+      <c r="J17" s="6">
+        <v>2937.87</v>
+      </c>
+      <c r="K17" s="6">
+        <v>184.2</v>
+      </c>
+      <c r="L17" s="6">
+        <v>2661.57</v>
+      </c>
+      <c r="M17" s="6">
+        <v>105.6</v>
+      </c>
+      <c r="N17" s="6"/>
+      <c r="O17" s="6"/>
+      <c r="P17" s="6"/>
+      <c r="Q17" s="6"/>
+      <c r="R17" s="6">
+        <v>2285.96</v>
+      </c>
+      <c r="S17" s="6">
+        <v>11.44</v>
+      </c>
+    </row>
+    <row r="18" spans="1:19" x14ac:dyDescent="0.3">
+      <c r="A18" t="s">
+        <v>30</v>
+      </c>
+      <c r="B18" s="6">
+        <v>1106.19</v>
+      </c>
+      <c r="C18" s="6">
+        <v>65.510000000000005</v>
+      </c>
+      <c r="D18" s="6">
+        <v>1133.8800000000001</v>
+      </c>
+      <c r="E18" s="6">
+        <v>93.27</v>
+      </c>
+      <c r="F18" s="6">
+        <v>989.56899999999996</v>
+      </c>
+      <c r="G18" s="6">
+        <v>52.6</v>
+      </c>
+      <c r="H18" s="6">
+        <v>894.55100000000004</v>
+      </c>
+      <c r="I18" s="6">
+        <v>61.52</v>
+      </c>
+      <c r="J18" s="6">
+        <v>1002.81</v>
+      </c>
+      <c r="K18" s="6">
+        <v>56.07</v>
+      </c>
+      <c r="L18" s="6">
+        <v>892.048</v>
+      </c>
+      <c r="M18" s="6">
+        <v>46.27</v>
+      </c>
+      <c r="N18" s="6"/>
+      <c r="O18" s="6"/>
+      <c r="P18" s="6"/>
+      <c r="Q18" s="6"/>
+      <c r="R18" s="6">
+        <v>619.279</v>
+      </c>
+      <c r="S18" s="6">
+        <v>3.2890000000000001</v>
+      </c>
+    </row>
+    <row r="19" spans="1:19" x14ac:dyDescent="0.3">
+      <c r="A19" t="s">
+        <v>31</v>
+      </c>
+      <c r="B19" s="6">
+        <v>2785.26</v>
+      </c>
+      <c r="C19" s="6">
+        <v>39.11</v>
+      </c>
+      <c r="D19" s="6">
+        <v>2652.96</v>
+      </c>
+      <c r="E19" s="6">
+        <v>62.6</v>
+      </c>
+      <c r="F19" s="6">
+        <v>2737.25</v>
+      </c>
+      <c r="G19" s="6">
+        <v>9.4079999999999995</v>
+      </c>
+      <c r="H19" s="6">
+        <v>2561.13</v>
+      </c>
+      <c r="I19" s="6">
+        <v>14.68</v>
+      </c>
+      <c r="J19" s="6">
+        <v>2725.59</v>
+      </c>
+      <c r="K19" s="6">
+        <v>16.309999999999999</v>
+      </c>
+      <c r="L19" s="6">
+        <v>2556.17</v>
+      </c>
+      <c r="M19" s="6">
+        <v>31.92</v>
+      </c>
+      <c r="N19" s="6"/>
+      <c r="O19" s="6"/>
+      <c r="P19" s="6"/>
+      <c r="Q19" s="6"/>
+      <c r="R19" s="6">
+        <v>2115.15</v>
+      </c>
+      <c r="S19" s="6">
+        <v>0.75600000000000001</v>
+      </c>
+    </row>
+    <row r="20" spans="1:19" x14ac:dyDescent="0.3">
+      <c r="A20" t="s">
+        <v>32</v>
+      </c>
+      <c r="B20" s="6">
+        <v>1038.4100000000001</v>
+      </c>
+      <c r="C20" s="6">
+        <v>7.3579999999999997</v>
+      </c>
+      <c r="D20" s="6">
+        <v>1142.6099999999999</v>
+      </c>
+      <c r="E20" s="6">
+        <v>106</v>
+      </c>
+      <c r="F20" s="6">
+        <v>949.89800000000002</v>
+      </c>
+      <c r="G20" s="6">
+        <v>3.7389999999999999</v>
+      </c>
+      <c r="H20" s="6">
+        <v>809.73699999999997</v>
+      </c>
+      <c r="I20" s="6">
+        <v>7.633</v>
+      </c>
+      <c r="J20" s="6">
+        <v>958.697</v>
+      </c>
+      <c r="K20" s="6">
+        <v>21.99</v>
+      </c>
+      <c r="L20" s="6">
+        <v>841.14599999999996</v>
+      </c>
+      <c r="M20" s="6">
+        <v>68.8</v>
+      </c>
+      <c r="N20" s="6"/>
+      <c r="O20" s="6"/>
+      <c r="P20" s="6"/>
+      <c r="Q20" s="6"/>
+      <c r="R20" s="6">
+        <v>542.00300000000004</v>
+      </c>
+      <c r="S20" s="6">
+        <v>0.77070000000000005</v>
+      </c>
+    </row>
+    <row r="21" spans="1:19" x14ac:dyDescent="0.3">
+      <c r="A21" t="s">
+        <v>33</v>
+      </c>
+      <c r="B21" s="6">
+        <v>4084.39</v>
+      </c>
+      <c r="C21" s="6">
+        <v>36.270000000000003</v>
+      </c>
+      <c r="D21" s="6">
+        <v>4440.4399999999996</v>
+      </c>
+      <c r="E21" s="6">
+        <v>422</v>
+      </c>
+      <c r="F21" s="6">
+        <v>4023.56</v>
+      </c>
+      <c r="G21" s="6">
+        <v>18.77</v>
+      </c>
+      <c r="H21" s="6">
+        <v>3916.35</v>
+      </c>
+      <c r="I21" s="6">
+        <v>26.49</v>
+      </c>
+      <c r="J21" s="6">
+        <v>4019.71</v>
+      </c>
+      <c r="K21" s="6">
+        <v>24.24</v>
+      </c>
+      <c r="L21" s="6">
+        <v>3950.88</v>
+      </c>
+      <c r="M21" s="6">
+        <v>12.9</v>
+      </c>
+      <c r="N21" s="6"/>
+      <c r="O21" s="6"/>
+      <c r="P21" s="6"/>
+      <c r="Q21" s="6"/>
+      <c r="R21" s="6">
+        <v>3547.4</v>
+      </c>
+      <c r="S21" s="6">
+        <v>8.2409999999999997</v>
+      </c>
+    </row>
+    <row r="22" spans="1:19" x14ac:dyDescent="0.3">
+      <c r="A22" t="s">
+        <v>34</v>
+      </c>
+      <c r="B22" s="6">
+        <v>4107.3599999999997</v>
+      </c>
+      <c r="C22" s="6">
+        <v>25.24</v>
+      </c>
+      <c r="D22" s="6">
+        <v>4408.1000000000004</v>
+      </c>
+      <c r="E22" s="6">
+        <v>384.1</v>
+      </c>
+      <c r="F22" s="6">
+        <v>4373.6000000000004</v>
+      </c>
+      <c r="G22" s="6">
+        <v>73.36</v>
+      </c>
+      <c r="H22" s="6">
+        <v>3940.51</v>
+      </c>
+      <c r="I22" s="6">
+        <v>38.520000000000003</v>
+      </c>
+      <c r="J22" s="6">
+        <v>4340.3100000000004</v>
+      </c>
+      <c r="K22" s="6">
+        <v>37.79</v>
+      </c>
+      <c r="L22" s="6">
+        <v>3941.11</v>
+      </c>
+      <c r="M22" s="6">
+        <v>23.57</v>
+      </c>
+      <c r="N22" s="6"/>
+      <c r="O22" s="6"/>
+      <c r="P22" s="6"/>
+      <c r="Q22" s="6"/>
+      <c r="R22" s="6">
+        <v>3512.47</v>
+      </c>
+      <c r="S22" s="6">
+        <v>5.4960000000000004</v>
+      </c>
+    </row>
+  </sheetData>
+  <mergeCells count="18">
+    <mergeCell ref="F4:I4"/>
+    <mergeCell ref="B1:M1"/>
+    <mergeCell ref="B2:M2"/>
+    <mergeCell ref="B3:M3"/>
+    <mergeCell ref="J4:M4"/>
+    <mergeCell ref="B5:C5"/>
+    <mergeCell ref="D5:E5"/>
+    <mergeCell ref="N5:O5"/>
+    <mergeCell ref="P5:Q5"/>
+    <mergeCell ref="F5:G5"/>
+    <mergeCell ref="H5:I5"/>
+    <mergeCell ref="J5:K5"/>
+    <mergeCell ref="L5:M5"/>
+    <mergeCell ref="N1:Q1"/>
+    <mergeCell ref="R1:U1"/>
+    <mergeCell ref="R2:U2"/>
+    <mergeCell ref="N3:Q3"/>
+    <mergeCell ref="R3:U3"/>
+  </mergeCells>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:U22"/>
+  <sheetViews>
+    <sheetView topLeftCell="B1" workbookViewId="0">
+      <selection activeCell="H37" sqref="H37"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <cols>
+    <col min="1" max="1" width="80.88671875" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="14.109375" customWidth="1"/>
+    <col min="3" max="3" width="8.77734375" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="14.77734375" customWidth="1"/>
+    <col min="6" max="6" width="13.5546875" customWidth="1"/>
+    <col min="8" max="8" width="13.77734375" customWidth="1"/>
+    <col min="9" max="9" width="9.109375" customWidth="1"/>
+    <col min="14" max="14" width="12.88671875" customWidth="1"/>
+    <col min="16" max="16" width="10.44140625" customWidth="1"/>
+    <col min="18" max="19" width="12.88671875" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:21" x14ac:dyDescent="0.3">
+      <c r="B1" s="11" t="s">
+        <v>44</v>
+      </c>
+      <c r="C1" s="11"/>
+      <c r="D1" s="11"/>
+      <c r="E1" s="11"/>
+      <c r="F1" s="11"/>
+      <c r="G1" s="11"/>
+      <c r="H1" s="11"/>
+      <c r="I1" s="11"/>
+      <c r="J1" s="11"/>
+      <c r="K1" s="11"/>
+      <c r="L1" s="11"/>
+      <c r="M1" s="11"/>
+      <c r="N1" s="11" t="s">
+        <v>47</v>
+      </c>
+      <c r="O1" s="11"/>
+      <c r="P1" s="11"/>
+      <c r="Q1" s="11"/>
+      <c r="R1" s="11" t="s">
+        <v>43</v>
+      </c>
+      <c r="S1" s="11"/>
+      <c r="T1" s="11"/>
+      <c r="U1" s="11"/>
+    </row>
+    <row r="2" spans="1:21" x14ac:dyDescent="0.3">
+      <c r="B2" s="11" t="s">
+        <v>38</v>
+      </c>
+      <c r="C2" s="11"/>
+      <c r="D2" s="11"/>
+      <c r="E2" s="11"/>
+      <c r="F2" s="11"/>
+      <c r="G2" s="11"/>
+      <c r="H2" s="11"/>
+      <c r="I2" s="11"/>
+      <c r="J2" s="11"/>
+      <c r="K2" s="11"/>
+      <c r="L2" s="11"/>
+      <c r="M2" s="11"/>
+      <c r="N2" s="9"/>
+      <c r="O2" s="9"/>
+      <c r="P2" s="9"/>
+      <c r="Q2" s="9"/>
+      <c r="R2" s="11" t="s">
+        <v>42</v>
+      </c>
+      <c r="S2" s="11"/>
+      <c r="T2" s="11"/>
+      <c r="U2" s="11"/>
+    </row>
+    <row r="3" spans="1:21" x14ac:dyDescent="0.3">
+      <c r="B3" s="11" t="s">
+        <v>39</v>
+      </c>
+      <c r="C3" s="11"/>
+      <c r="D3" s="11"/>
+      <c r="E3" s="11"/>
+      <c r="F3" s="11"/>
+      <c r="G3" s="11"/>
+      <c r="H3" s="11"/>
+      <c r="I3" s="11"/>
+      <c r="J3" s="11"/>
+      <c r="K3" s="11"/>
+      <c r="L3" s="11"/>
+      <c r="M3" s="11"/>
+      <c r="N3" s="11" t="s">
+        <v>39</v>
+      </c>
+      <c r="O3" s="11"/>
+      <c r="P3" s="11"/>
+      <c r="Q3" s="11"/>
+      <c r="R3" s="11" t="s">
+        <v>45</v>
+      </c>
+      <c r="S3" s="11"/>
+      <c r="T3" s="11"/>
+      <c r="U3" s="11"/>
+    </row>
+    <row r="4" spans="1:21" x14ac:dyDescent="0.3">
+      <c r="B4" s="9"/>
+      <c r="C4" s="9"/>
+      <c r="D4" s="9"/>
+      <c r="E4" s="9"/>
+      <c r="F4" s="11" t="s">
+        <v>51</v>
+      </c>
+      <c r="G4" s="11"/>
+      <c r="H4" s="11"/>
+      <c r="I4" s="11"/>
+      <c r="J4" s="11" t="s">
+        <v>52</v>
+      </c>
+      <c r="K4" s="11"/>
+      <c r="L4" s="11"/>
+      <c r="M4" s="11"/>
+      <c r="N4" s="9"/>
+      <c r="O4" s="9"/>
+      <c r="P4" s="9"/>
+      <c r="Q4" s="9"/>
+      <c r="R4" s="9"/>
+      <c r="S4" s="9"/>
+      <c r="T4" s="9"/>
+      <c r="U4" s="9"/>
+    </row>
+    <row r="5" spans="1:21" x14ac:dyDescent="0.3">
+      <c r="B5" s="11" t="s">
+        <v>41</v>
+      </c>
+      <c r="C5" s="11"/>
+      <c r="D5" s="11" t="s">
+        <v>40</v>
+      </c>
+      <c r="E5" s="11"/>
+      <c r="F5" s="11" t="s">
+        <v>41</v>
+      </c>
+      <c r="G5" s="11"/>
+      <c r="H5" s="11" t="s">
+        <v>40</v>
+      </c>
+      <c r="I5" s="11"/>
+      <c r="J5" s="11" t="s">
+        <v>41</v>
+      </c>
+      <c r="K5" s="11"/>
+      <c r="L5" s="11" t="s">
+        <v>40</v>
+      </c>
+      <c r="M5" s="11"/>
+      <c r="N5" s="11" t="s">
+        <v>41</v>
+      </c>
+      <c r="O5" s="11"/>
+      <c r="P5" s="11" t="s">
+        <v>40</v>
+      </c>
+      <c r="Q5" s="11"/>
+    </row>
+    <row r="6" spans="1:21" x14ac:dyDescent="0.3">
+      <c r="A6" t="s">
+        <v>35</v>
+      </c>
+      <c r="B6" s="9" t="s">
+        <v>49</v>
+      </c>
+      <c r="C6" s="9" t="s">
+        <v>50</v>
+      </c>
+      <c r="D6" s="9" t="s">
+        <v>49</v>
+      </c>
+      <c r="E6" s="9" t="s">
+        <v>50</v>
+      </c>
+      <c r="F6" s="9" t="s">
+        <v>49</v>
+      </c>
+      <c r="G6" s="9" t="s">
+        <v>50</v>
+      </c>
+      <c r="H6" s="9" t="s">
+        <v>49</v>
+      </c>
+      <c r="I6" s="9" t="s">
+        <v>50</v>
+      </c>
+      <c r="J6" s="9" t="s">
+        <v>49</v>
+      </c>
+      <c r="K6" s="9" t="s">
+        <v>50</v>
+      </c>
+      <c r="L6" s="9" t="s">
+        <v>49</v>
+      </c>
+      <c r="M6" s="9" t="s">
+        <v>50</v>
+      </c>
+      <c r="N6" s="9" t="s">
+        <v>49</v>
+      </c>
+      <c r="O6" s="9" t="s">
+        <v>50</v>
+      </c>
+      <c r="P6" s="9" t="s">
+        <v>49</v>
+      </c>
+      <c r="Q6" s="9" t="s">
+        <v>50</v>
+      </c>
+      <c r="R6" s="9" t="s">
+        <v>49</v>
+      </c>
+      <c r="S6" s="9" t="s">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="7" spans="1:21" x14ac:dyDescent="0.3">
+      <c r="A7" t="s">
+        <v>19</v>
+      </c>
+      <c r="B7" s="6">
+        <v>1329.2</v>
+      </c>
+      <c r="C7" s="6">
+        <v>27.94</v>
+      </c>
+      <c r="D7" s="6">
+        <v>1371.61</v>
+      </c>
+      <c r="E7" s="6">
+        <v>25.04</v>
+      </c>
+      <c r="F7" s="6">
+        <v>1322.08</v>
+      </c>
+      <c r="G7" s="6">
+        <v>10.79</v>
+      </c>
+      <c r="H7" s="6">
+        <v>1372.45</v>
+      </c>
+      <c r="I7" s="6">
+        <v>12.52</v>
+      </c>
+      <c r="J7" s="6">
+        <v>1321.94</v>
+      </c>
+      <c r="K7" s="6">
+        <v>7.117</v>
+      </c>
+      <c r="L7" s="6">
+        <v>1400.14</v>
+      </c>
+      <c r="M7" s="6">
+        <v>23.35</v>
+      </c>
+      <c r="N7" s="6"/>
+      <c r="O7" s="6"/>
+      <c r="R7" s="6">
+        <v>1399.54</v>
+      </c>
+      <c r="S7" s="6">
+        <v>10.9</v>
+      </c>
+    </row>
+    <row r="8" spans="1:21" x14ac:dyDescent="0.3">
+      <c r="A8" t="s">
+        <v>20</v>
+      </c>
+      <c r="B8" s="6">
+        <v>475.17899999999997</v>
+      </c>
+      <c r="C8" s="6">
+        <v>2.6459999999999999</v>
+      </c>
+      <c r="D8" s="6">
+        <v>583.16099999999994</v>
+      </c>
+      <c r="E8" s="6">
+        <v>6.585</v>
+      </c>
+      <c r="F8" s="6">
+        <v>340.339</v>
+      </c>
+      <c r="G8" s="6">
+        <v>2.8180000000000001</v>
+      </c>
+      <c r="H8" s="6">
+        <v>388.73200000000003</v>
+      </c>
+      <c r="I8" s="6">
+        <v>2.6230000000000002</v>
+      </c>
+      <c r="J8" s="6">
+        <v>339.49299999999999</v>
+      </c>
+      <c r="K8" s="6">
+        <v>4.1180000000000003</v>
+      </c>
+      <c r="L8" s="6">
+        <v>332.9</v>
+      </c>
+      <c r="M8" s="6">
+        <v>3.5419999999999998</v>
+      </c>
+      <c r="R8" s="6">
+        <v>302.964</v>
+      </c>
+      <c r="S8" s="6">
+        <v>10.55</v>
+      </c>
+    </row>
+    <row r="9" spans="1:21" x14ac:dyDescent="0.3">
+      <c r="A9" t="s">
+        <v>21</v>
+      </c>
+      <c r="B9" s="6">
+        <v>1320.92</v>
+      </c>
+      <c r="C9" s="6">
+        <v>17.04</v>
+      </c>
+      <c r="D9" s="6">
+        <v>1380.5</v>
+      </c>
+      <c r="E9" s="6">
+        <v>13.83</v>
+      </c>
+      <c r="F9" s="6">
+        <v>1338.92</v>
+      </c>
+      <c r="G9" s="6">
+        <v>33.450000000000003</v>
+      </c>
+      <c r="H9" s="6">
+        <v>1352.84</v>
+      </c>
+      <c r="I9" s="6">
+        <v>8.66</v>
+      </c>
+      <c r="J9" s="6">
+        <v>1328.66</v>
+      </c>
+      <c r="K9" s="6">
+        <v>13.43</v>
+      </c>
+      <c r="L9" s="6">
+        <v>1358.78</v>
+      </c>
+      <c r="M9" s="6">
+        <v>7.5810000000000004</v>
+      </c>
+      <c r="R9" s="6">
+        <v>1313.2</v>
+      </c>
+      <c r="S9" s="6">
+        <v>1.407</v>
+      </c>
+    </row>
+    <row r="10" spans="1:21" x14ac:dyDescent="0.3">
+      <c r="A10" t="s">
+        <v>22</v>
+      </c>
+      <c r="B10" s="6">
+        <v>474.34899999999999</v>
+      </c>
+      <c r="C10" s="6">
+        <v>6.0250000000000004</v>
+      </c>
+      <c r="D10" s="6">
+        <v>583.005</v>
+      </c>
+      <c r="E10" s="6">
+        <v>21.98</v>
+      </c>
+      <c r="F10" s="6">
+        <v>337.75200000000001</v>
+      </c>
+      <c r="G10" s="6">
+        <v>2.1829999999999998</v>
+      </c>
+      <c r="H10" s="6">
+        <v>385.35899999999998</v>
+      </c>
+      <c r="I10" s="6">
+        <v>15.55</v>
+      </c>
+      <c r="J10" s="6">
+        <v>337.089</v>
+      </c>
+      <c r="K10" s="6">
+        <v>1.7230000000000001</v>
+      </c>
+      <c r="L10" s="6">
+        <v>335.77800000000002</v>
+      </c>
+      <c r="M10" s="6">
+        <v>4.4329999999999998</v>
+      </c>
+      <c r="R10" s="6">
+        <v>300.86099999999999</v>
+      </c>
+      <c r="S10" s="6">
+        <v>4.7169999999999996</v>
+      </c>
+    </row>
+    <row r="11" spans="1:21" x14ac:dyDescent="0.3">
+      <c r="A11" t="s">
+        <v>23</v>
+      </c>
+      <c r="B11" s="6">
+        <v>1392.7</v>
+      </c>
+      <c r="C11" s="6">
+        <v>20.79</v>
+      </c>
+      <c r="D11" s="6">
+        <v>1395.88</v>
+      </c>
+      <c r="E11" s="6">
+        <v>28.77</v>
+      </c>
+      <c r="F11" s="6">
+        <v>1416.49</v>
+      </c>
+      <c r="G11" s="6">
+        <v>2.1669999999999998</v>
+      </c>
+      <c r="H11" s="6">
+        <v>1371.62</v>
+      </c>
+      <c r="I11" s="6">
+        <v>10.54</v>
+      </c>
+      <c r="J11" s="6">
+        <v>1419.54</v>
+      </c>
+      <c r="K11" s="6">
+        <v>12.82</v>
+      </c>
+      <c r="L11" s="6">
+        <v>1393.68</v>
+      </c>
+      <c r="M11" s="6">
+        <v>18.64</v>
+      </c>
+      <c r="R11" s="6">
+        <v>1129.69</v>
+      </c>
+      <c r="S11" s="6">
+        <v>7.4560000000000004</v>
+      </c>
+    </row>
+    <row r="12" spans="1:21" x14ac:dyDescent="0.3">
+      <c r="A12" t="s">
+        <v>24</v>
+      </c>
+      <c r="B12" s="6">
+        <v>539.25300000000004</v>
+      </c>
+      <c r="C12" s="6">
+        <v>6.1390000000000002</v>
+      </c>
+      <c r="D12" s="6">
+        <v>561.63099999999997</v>
+      </c>
+      <c r="E12" s="6">
+        <v>5.9610000000000003</v>
+      </c>
+      <c r="F12" s="6">
+        <v>422.911</v>
+      </c>
+      <c r="G12" s="6">
+        <v>12.04</v>
+      </c>
+      <c r="H12" s="6">
+        <v>409.57499999999999</v>
+      </c>
+      <c r="I12" s="6">
+        <v>8.89</v>
+      </c>
+      <c r="J12" s="6">
+        <v>423.36500000000001</v>
+      </c>
+      <c r="K12" s="6">
+        <v>9.9499999999999993</v>
+      </c>
+      <c r="L12" s="6">
+        <v>408.56799999999998</v>
+      </c>
+      <c r="M12" s="6">
+        <v>13</v>
+      </c>
+      <c r="R12" s="6">
+        <v>294.54599999999999</v>
+      </c>
+      <c r="S12" s="6">
+        <v>2.4689999999999999</v>
+      </c>
+    </row>
+    <row r="13" spans="1:21" x14ac:dyDescent="0.3">
+      <c r="A13" t="s">
+        <v>25</v>
+      </c>
+      <c r="B13" s="6">
+        <v>1377.73</v>
+      </c>
+      <c r="C13" s="6">
+        <v>16.47</v>
+      </c>
+      <c r="D13" s="6">
+        <v>1401.51</v>
+      </c>
+      <c r="E13" s="6">
+        <v>13.44</v>
+      </c>
+      <c r="F13" s="6">
+        <v>1370.59</v>
+      </c>
+      <c r="G13" s="6">
+        <v>10.31</v>
+      </c>
+      <c r="H13" s="6">
+        <v>1408.62</v>
+      </c>
+      <c r="I13" s="6">
+        <v>14.12</v>
+      </c>
+      <c r="J13" s="6">
+        <v>1372.97</v>
+      </c>
+      <c r="K13" s="6">
+        <v>19.18</v>
+      </c>
+      <c r="L13" s="6">
+        <v>1415.75</v>
+      </c>
+      <c r="M13" s="6">
+        <v>16.12</v>
+      </c>
+      <c r="R13" s="6">
+        <v>1149.96</v>
+      </c>
+      <c r="S13" s="6">
+        <v>1.603</v>
+      </c>
+    </row>
+    <row r="14" spans="1:21" x14ac:dyDescent="0.3">
+      <c r="A14" t="s">
+        <v>26</v>
+      </c>
+      <c r="B14" s="6">
+        <v>581.87599999999998</v>
+      </c>
+      <c r="C14" s="6">
+        <v>9.0549999999999997</v>
+      </c>
+      <c r="D14" s="6">
+        <v>636.74599999999998</v>
+      </c>
+      <c r="E14" s="6">
+        <v>6.4820000000000002</v>
+      </c>
+      <c r="F14" s="6">
+        <v>406.01499999999999</v>
+      </c>
+      <c r="G14" s="6">
+        <v>2.0569999999999999</v>
+      </c>
+      <c r="H14" s="6">
+        <v>436.44499999999999</v>
+      </c>
+      <c r="I14" s="6">
+        <v>3.5019999999999998</v>
+      </c>
+      <c r="J14" s="6">
+        <v>405.04500000000002</v>
+      </c>
+      <c r="K14" s="6">
+        <v>0.52849999999999997</v>
+      </c>
+      <c r="L14" s="6">
+        <v>426.32799999999997</v>
+      </c>
+      <c r="M14" s="6">
+        <v>3.9790000000000001</v>
+      </c>
+      <c r="R14" s="6">
+        <v>306.721</v>
+      </c>
+      <c r="S14" s="6">
+        <v>1.768</v>
+      </c>
+    </row>
+    <row r="15" spans="1:21" x14ac:dyDescent="0.3">
+      <c r="A15" t="s">
+        <v>27</v>
+      </c>
+      <c r="B15" s="6">
+        <v>1151</v>
+      </c>
+      <c r="C15" s="6">
+        <v>12.85</v>
+      </c>
+      <c r="D15" s="6">
+        <v>1136.93</v>
+      </c>
+      <c r="E15" s="6">
+        <v>9.2439999999999998</v>
+      </c>
+      <c r="F15" s="6">
+        <v>1131.6400000000001</v>
+      </c>
+      <c r="G15" s="6">
+        <v>8.8650000000000002</v>
+      </c>
+      <c r="H15" s="6">
+        <v>1133.26</v>
+      </c>
+      <c r="I15" s="6">
+        <v>7.0049999999999999</v>
+      </c>
+      <c r="J15" s="6">
+        <v>1133.8800000000001</v>
+      </c>
+      <c r="K15" s="6">
+        <v>18.190000000000001</v>
+      </c>
+      <c r="L15" s="6">
+        <v>1162.54</v>
+      </c>
+      <c r="M15" s="6">
+        <v>14.35</v>
+      </c>
+      <c r="R15" s="6">
+        <v>1076.6099999999999</v>
+      </c>
+      <c r="S15" s="6">
+        <v>0.5413</v>
+      </c>
+    </row>
+    <row r="16" spans="1:21" x14ac:dyDescent="0.3">
+      <c r="A16" t="s">
+        <v>28</v>
+      </c>
+      <c r="B16" s="6">
+        <v>437.83100000000002</v>
+      </c>
+      <c r="C16" s="6">
+        <v>18.010000000000002</v>
+      </c>
+      <c r="D16" s="6">
+        <v>304.71100000000001</v>
+      </c>
+      <c r="E16" s="6">
+        <v>1.5840000000000001</v>
+      </c>
+      <c r="F16" s="6">
+        <v>427.71699999999998</v>
+      </c>
+      <c r="G16" s="6">
+        <v>4.3390000000000004</v>
+      </c>
+      <c r="H16" s="6">
+        <v>304.96899999999999</v>
+      </c>
+      <c r="I16" s="6">
+        <v>1.488</v>
+      </c>
+      <c r="J16" s="6">
+        <v>433.65499999999997</v>
+      </c>
+      <c r="K16" s="6">
+        <v>1.429</v>
+      </c>
+      <c r="L16" s="6">
+        <v>310.10500000000002</v>
+      </c>
+      <c r="M16" s="6">
+        <v>1.6140000000000001</v>
+      </c>
+      <c r="R16" s="6">
+        <v>134.37799999999999</v>
+      </c>
+      <c r="S16" s="6">
+        <v>0.6633</v>
+      </c>
+    </row>
+    <row r="17" spans="1:19" x14ac:dyDescent="0.3">
+      <c r="A17" t="s">
+        <v>29</v>
+      </c>
+      <c r="B17" s="6">
+        <v>1443.8</v>
+      </c>
+      <c r="C17" s="6">
+        <v>11.21</v>
+      </c>
+      <c r="D17" s="6">
+        <v>1305.8699999999999</v>
+      </c>
+      <c r="E17" s="6">
+        <v>10.65</v>
+      </c>
+      <c r="F17" s="6">
+        <v>1466.95</v>
+      </c>
+      <c r="G17" s="6">
+        <v>16.93</v>
+      </c>
+      <c r="H17" s="6">
+        <v>1308.7</v>
+      </c>
+      <c r="I17" s="6">
+        <v>16.329999999999998</v>
+      </c>
+      <c r="J17" s="6">
+        <v>1471.56</v>
+      </c>
+      <c r="K17" s="6">
+        <v>30.63</v>
+      </c>
+      <c r="L17" s="6">
+        <v>1324.76</v>
+      </c>
+      <c r="M17" s="6">
+        <v>11.14</v>
+      </c>
+      <c r="R17" s="6">
+        <v>1269.44</v>
+      </c>
+      <c r="S17" s="6">
+        <v>6.3460000000000001</v>
+      </c>
+    </row>
+    <row r="18" spans="1:19" x14ac:dyDescent="0.3">
+      <c r="A18" t="s">
+        <v>30</v>
+      </c>
+      <c r="B18" s="6">
+        <v>471.149</v>
+      </c>
+      <c r="C18" s="6">
+        <v>8.3140000000000001</v>
+      </c>
+      <c r="D18" s="6">
+        <v>471.54399999999998</v>
+      </c>
+      <c r="E18" s="6">
+        <v>4.9809999999999999</v>
+      </c>
+      <c r="F18" s="6">
+        <v>326.51499999999999</v>
+      </c>
+      <c r="G18" s="6">
+        <v>7.3179999999999996</v>
+      </c>
+      <c r="H18" s="6">
+        <v>270.73899999999998</v>
+      </c>
+      <c r="I18" s="6">
+        <v>15.54</v>
+      </c>
+      <c r="J18" s="6">
+        <v>321.858</v>
+      </c>
+      <c r="K18" s="6">
+        <v>3.6440000000000001</v>
+      </c>
+      <c r="L18" s="6">
+        <v>270.85899999999998</v>
+      </c>
+      <c r="M18" s="6">
+        <v>14.88</v>
+      </c>
+      <c r="R18" s="6">
+        <v>170.28800000000001</v>
+      </c>
+      <c r="S18" s="6">
+        <v>0.34689999999999999</v>
+      </c>
+    </row>
+    <row r="19" spans="1:19" x14ac:dyDescent="0.3">
+      <c r="A19" t="s">
+        <v>31</v>
+      </c>
+      <c r="B19" s="6">
+        <v>1410.19</v>
+      </c>
+      <c r="C19" s="6">
+        <v>13.07</v>
+      </c>
+      <c r="D19" s="6">
+        <v>1330.09</v>
+      </c>
+      <c r="E19" s="6">
+        <v>18.68</v>
+      </c>
+      <c r="F19" s="6">
+        <v>1437.72</v>
+      </c>
+      <c r="G19" s="6">
+        <v>27.54</v>
+      </c>
+      <c r="H19" s="6">
+        <v>1338.78</v>
+      </c>
+      <c r="I19" s="6">
+        <v>21.13</v>
+      </c>
+      <c r="J19" s="6">
+        <v>1428.64</v>
+      </c>
+      <c r="K19" s="6">
+        <v>8.0030000000000001</v>
+      </c>
+      <c r="L19" s="6">
+        <v>1326.11</v>
+      </c>
+      <c r="M19" s="6">
+        <v>8.6839999999999993</v>
+      </c>
+      <c r="R19" s="6">
+        <v>1297.02</v>
+      </c>
+      <c r="S19" s="6">
+        <v>3.21</v>
+      </c>
+    </row>
+    <row r="20" spans="1:19" x14ac:dyDescent="0.3">
+      <c r="A20" t="s">
+        <v>32</v>
+      </c>
+      <c r="B20" s="6">
+        <v>467.84300000000002</v>
+      </c>
+      <c r="C20" s="6">
+        <v>5.76</v>
+      </c>
+      <c r="D20" s="6">
+        <v>470.81799999999998</v>
+      </c>
+      <c r="E20" s="6">
+        <v>5.0780000000000003</v>
+      </c>
+      <c r="F20" s="6">
+        <v>324.19400000000002</v>
+      </c>
+      <c r="G20" s="6">
+        <v>3.0379999999999998</v>
+      </c>
+      <c r="H20" s="6">
+        <v>255.608</v>
+      </c>
+      <c r="I20" s="6">
+        <v>0.86240000000000006</v>
+      </c>
+      <c r="J20" s="6">
+        <v>317.77199999999999</v>
+      </c>
+      <c r="K20" s="6">
+        <v>1.18</v>
+      </c>
+      <c r="L20" s="6">
+        <v>255.89699999999999</v>
+      </c>
+      <c r="M20" s="6">
+        <v>2.4620000000000002</v>
+      </c>
+      <c r="R20" s="6">
+        <v>173.244</v>
+      </c>
+      <c r="S20" s="6">
+        <v>0.52170000000000005</v>
+      </c>
+    </row>
+    <row r="21" spans="1:19" x14ac:dyDescent="0.3">
+      <c r="A21" t="s">
+        <v>33</v>
+      </c>
+      <c r="B21" s="6">
+        <v>412.714</v>
+      </c>
+      <c r="C21" s="6">
+        <v>5.585</v>
+      </c>
+      <c r="D21" s="6">
+        <v>508.995</v>
+      </c>
+      <c r="E21" s="6">
+        <v>4.6130000000000004</v>
+      </c>
+      <c r="F21" s="6">
+        <v>312.06400000000002</v>
+      </c>
+      <c r="G21" s="6">
+        <v>1.6930000000000001</v>
+      </c>
+      <c r="H21" s="6">
+        <v>323.56299999999999</v>
+      </c>
+      <c r="I21" s="6">
+        <v>2.46</v>
+      </c>
+      <c r="J21" s="6">
+        <v>313.59300000000002</v>
+      </c>
+      <c r="K21" s="6">
+        <v>3.6949999999999998</v>
+      </c>
+      <c r="L21" s="6">
+        <v>325.41399999999999</v>
+      </c>
+      <c r="M21" s="6">
+        <v>1.2809999999999999</v>
+      </c>
+      <c r="R21" s="6">
+        <v>191.03299999999999</v>
+      </c>
+      <c r="S21" s="6">
+        <v>1.016</v>
+      </c>
+    </row>
+    <row r="22" spans="1:19" x14ac:dyDescent="0.3">
+      <c r="A22" t="s">
+        <v>34</v>
+      </c>
+      <c r="B22" s="6">
+        <v>406.96</v>
+      </c>
+      <c r="C22" s="6">
+        <v>5.3380000000000001</v>
+      </c>
+      <c r="D22" s="6">
+        <v>490.75799999999998</v>
+      </c>
+      <c r="E22" s="6">
+        <v>18.510000000000002</v>
+      </c>
+      <c r="F22" s="6">
+        <v>284.33800000000002</v>
+      </c>
+      <c r="G22" s="6">
+        <v>1.9019999999999999</v>
+      </c>
+      <c r="H22" s="6">
+        <v>236.26</v>
+      </c>
+      <c r="I22" s="6">
+        <v>1.387</v>
+      </c>
+      <c r="J22" s="6">
+        <v>284.851</v>
+      </c>
+      <c r="K22" s="6">
+        <v>1.5820000000000001</v>
+      </c>
+      <c r="L22" s="6">
+        <v>240.036</v>
+      </c>
+      <c r="M22" s="6">
+        <v>0.90759999999999996</v>
+      </c>
+      <c r="R22" s="6">
+        <v>232.67099999999999</v>
+      </c>
+      <c r="S22" s="6">
+        <v>5.0629999999999997</v>
+      </c>
+    </row>
+  </sheetData>
+  <mergeCells count="18">
+    <mergeCell ref="N5:O5"/>
+    <mergeCell ref="P5:Q5"/>
+    <mergeCell ref="F4:I4"/>
+    <mergeCell ref="J4:M4"/>
+    <mergeCell ref="B5:C5"/>
+    <mergeCell ref="D5:E5"/>
+    <mergeCell ref="F5:G5"/>
+    <mergeCell ref="H5:I5"/>
+    <mergeCell ref="J5:K5"/>
+    <mergeCell ref="L5:M5"/>
+    <mergeCell ref="B1:M1"/>
+    <mergeCell ref="N1:Q1"/>
+    <mergeCell ref="R1:U1"/>
+    <mergeCell ref="B2:M2"/>
+    <mergeCell ref="R2:U2"/>
+    <mergeCell ref="B3:M3"/>
+    <mergeCell ref="N3:Q3"/>
+    <mergeCell ref="R3:U3"/>
+  </mergeCells>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
+</worksheet>
 </file>
</xml_diff>